<commit_message>
Write initial document for osrm graph partition.
</commit_message>
<xml_diff>
--- a/routing_basic/resource/pictures/temp.xlsx
+++ b/routing_basic/resource/pictures/temp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xunliu/Desktop/git/direction/direction/routing/research/routing_basic/resource/pictures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xunliu/Desktop/git/telenav/open-source-spec/routing_basic/resource/pictures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180694D7-CFD5-1C47-BC8D-CCF4E41134FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BE96C2-739B-3E4B-B6C9-B65224C7AE23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="4140" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4497,6 +4497,115 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A2AF1E1-8738-F942-84BE-4BBE4B1C950B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="4057650"/>
+          <a:ext cx="1676400" cy="25400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66101219-2BA6-A048-BBFE-D285AA626D5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4292600" y="4108450"/>
+          <a:ext cx="1676400" cy="25400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5121,7 +5230,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="BD37" sqref="BD37"/>
+      <selection activeCell="AZ23" sqref="AZ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>